<commit_message>
- Progressed work tasks
</commit_message>
<xml_diff>
--- a/Engines/Resources/Template.xlsx
+++ b/Engines/Resources/Template.xlsx
@@ -178,7 +178,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -208,6 +208,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="17" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -299,7 +300,7 @@
             <c:numRef>
               <c:f>DataHid!$C$6:$O$6</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
@@ -364,7 +365,7 @@
             <c:numRef>
               <c:f>DataHid!$C$7:$O$7</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
@@ -415,7 +416,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -438,6 +439,7 @@
         <c:axId val="728351648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -489,6 +491,7 @@
         <c:axId val="526976032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -673,7 +676,7 @@
             <c:numRef>
               <c:f>DataHid!$C$11:$P$11</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
               </c:numCache>
             </c:numRef>
@@ -738,7 +741,7 @@
             <c:numRef>
               <c:f>DataHid!$C$12:$P$12</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
               </c:numCache>
             </c:numRef>
@@ -789,7 +792,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -812,6 +815,7 @@
         <c:axId val="805123168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -863,6 +867,7 @@
         <c:axId val="1163826944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -4068,8 +4073,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="664263" y="8336445"/>
-          <a:ext cx="3456000" cy="584392"/>
+          <a:off x="673131" y="8336117"/>
+          <a:ext cx="3512165" cy="584392"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4120,7 +4125,31 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> ventas de {MONTH} han {VERB_1} en {PER_1}%, respecto al promedio de los 3 meses previos. Ad</a:t>
+            <a:t> ventas de {MONTH} se {VERB_1} {PER_1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="0" u="sng" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>},</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> respecto al promedio de los 3 meses previos. /Ad</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" baseline="0">
@@ -4144,7 +4173,7 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>, hubo un {VERB_2} del {PER_2}% respecto al mismo mes del año anterior.</a:t>
+            <a:t>, {VERB_2} {PER_2} respecto al mismo mes del año anterior.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="800" b="0">
             <a:solidFill>
@@ -4163,13 +4192,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
+      <xdr:colOff>21583</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>59220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
+      <xdr:colOff>40633</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>39342</xdr:rowOff>
     </xdr:to>
@@ -4182,8 +4211,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4724399" y="8336445"/>
-          <a:ext cx="3457575" cy="551622"/>
+          <a:off x="4803790" y="8336117"/>
+          <a:ext cx="3513740" cy="551622"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4234,7 +4263,7 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> de tus clientes en {PER_1}% respecto al promedio de los ultimos 3 meses. Sin embargo tuviste un {VERB_2} del {PER_2}% respecto al mismo mes del año anterior.</a:t>
+            <a:t> de tus clientes {PER_1} respecto al promedio de los ultimos 3 meses. /Sin embargo tuviste {VERB_2} {PER_2} respecto al mismo mes del año anterior.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="800" b="0">
             <a:solidFill>
@@ -4433,7 +4462,7 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> clientes prefieren visitarte los días {DAYS}. </a:t>
+            <a:t> clientes prefieren visitarte los {DAYS}. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4448,7 +4477,7 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Podrías realizar campañas para atraer su atención en los días más bajos.</a:t>
+            <a:t>/Podrías realizar campañas para atraer su atención en los días más bajos.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="800">
             <a:solidFill>
@@ -7717,6 +7746,138 @@
             </a:solidFill>
             <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>121338</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>178447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>140248</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>13794</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="G2_FINAL"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="673131" y="8836344"/>
+          <a:ext cx="3513600" cy="216347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>{}</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>21653</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>178447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>40563</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>13794</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="G3_FINAL"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4803860" y="8836344"/>
+          <a:ext cx="3513600" cy="216347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>{}</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -12200,15 +12361,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -12258,22 +12419,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12294,8 +12455,9 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12303,20 +12465,26 @@
         <v>0</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12324,30 +12492,36 @@
         <v>1</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -12368,8 +12542,9 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -12377,20 +12552,25 @@
         <v>2</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -12398,25 +12578,30 @@
         <v>3</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -12424,7 +12609,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -12451,7 +12636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
- Fixed minor bugs.
</commit_message>
<xml_diff>
--- a/Engines/Resources/Template.xlsx
+++ b/Engines/Resources/Template.xlsx
@@ -468,7 +468,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -511,7 +511,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -844,7 +844,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -887,7 +887,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3062,13 +3062,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>146540</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3091,8 +3091,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="371476" y="390524"/>
-          <a:ext cx="8096249" cy="12792075"/>
+          <a:off x="375872" y="390525"/>
+          <a:ext cx="8196628" cy="12797938"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3906,13 +3906,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>37735</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>28942</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3938,13 +3938,13 @@
       <xdr:col>27</xdr:col>
       <xdr:colOff>108975</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
       <xdr:colOff>100575</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>103200</xdr:rowOff>
+      <xdr:rowOff>85574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4125,10 +4125,10 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> ventas de {MONTH} se {VERB_1} {PER_1</a:t>
+            <a:t> ventas de {MONTH} se {VERB_1} {</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="800" b="0" u="sng" baseline="0">
+            <a:rPr lang="en-US" sz="800" b="0" u="none" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4137,7 +4137,7 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>},</a:t>
+            <a:t>PER_1}, </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="800" b="0" baseline="0">
@@ -4149,7 +4149,7 @@
               </a:solidFill>
               <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> respecto al promedio de los 3 meses previos. /Ad</a:t>
+            <a:t>respecto al promedio de los 3 meses previos. /Ad</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" baseline="0">
@@ -6123,28 +6123,30 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>150818</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>6849</xdr:rowOff>
+      <xdr:colOff>169868</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>130039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>20706</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>43484</xdr:rowOff>
+      <xdr:colOff>39756</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>102044</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="78" name="ADVICE_GRAPHIC3"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="697470" y="12662675"/>
-          <a:ext cx="6429714" cy="417635"/>
+          <a:off x="713490" y="12401027"/>
+          <a:ext cx="6393351" cy="353005"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6171,12 +6173,12 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="700" b="1" i="1">
+            <a:rPr lang="en-US" sz="650" b="1" i="1">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -6204,7 +6206,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="700" b="1" i="1">
+            <a:rPr lang="en-US" sz="650" b="1" i="1">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -6215,7 +6217,7 @@
             </a:rPr>
             <a:t>2. Transacciones realizadas por negocios ubicados en la misma zona y giro.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="700" b="1" i="1">
+          <a:endParaRPr lang="en-US" sz="650" b="1" i="1">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -7600,15 +7602,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>103020</xdr:colOff>
+      <xdr:colOff>112313</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>82833</xdr:rowOff>
+      <xdr:rowOff>59602</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>75141</xdr:colOff>
+      <xdr:colOff>84434</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>41016</xdr:rowOff>
+      <xdr:rowOff>17785</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7619,8 +7621,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2126261" y="3787730"/>
-          <a:ext cx="156052" cy="148683"/>
+          <a:off x="2105593" y="3758090"/>
+          <a:ext cx="153329" cy="148683"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7677,15 +7679,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>26949</xdr:colOff>
+      <xdr:colOff>31595</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>26949</xdr:rowOff>
+      <xdr:rowOff>17657</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>180278</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3717</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>175632</xdr:rowOff>
+      <xdr:rowOff>166340</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7696,7 +7698,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2382644" y="4487437"/>
+          <a:off x="2387290" y="4478145"/>
           <a:ext cx="153329" cy="148683"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7883,6 +7885,123 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>173647</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>31705</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>145072</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>102044</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="FINALCOND"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="717269" y="12683693"/>
+          <a:ext cx="6494888" cy="260839"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="550">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Esta información mensual se podrá enviar hasta el 30 de Mayo y es totalmente gratuita. Los datos que se muestran en la hoja informativa hacen referencia a un determinado mes calendario y </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="550">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>son de carácter estadístico, en base al comportamiento mensual del negocio y del mercado, por lo tanto, su contenido no deberá ser empleado como documento oficial o comparado con el documento </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="550">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>autorizado (DA) enviado por La Compañía Peruana de Medios de Pago S.A.C. En caso de necesitar información adicional, contactar a nuestra central telefónica al número 01 614-9800</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="550">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="500">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:latin typeface="Trade Gothic LT Std" panose="020B0503020502020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7891,15 +8010,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>158869</xdr:colOff>
+      <xdr:colOff>164224</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7922,15 +8041,15 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="333375" y="400051"/>
-          <a:ext cx="8112244" cy="12782550"/>
+          <a:off x="323850" y="400050"/>
+          <a:ext cx="8127124" cy="12773025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -8237,7 +8356,9 @@
   </sheetPr>
   <dimension ref="A1:BB73"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="106" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A61" zoomScale="205" zoomScaleNormal="106" zoomScaleSheetLayoutView="205" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12329,7 +12450,7 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -12337,9 +12458,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A57:A69"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12354,7 +12480,7 @@
     <row r="69" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -12364,7 +12490,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>